<commit_message>
procida exercise own solution
</commit_message>
<xml_diff>
--- a/week5/procida_v1/work/procida_mål.xlsx
+++ b/week5/procida_v1/work/procida_mål.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11209"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isab7099/Documents/websites/week5/procida_v1/work/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D66930E8-5B57-2941-85AC-232E8C349C66}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="4320" yWindow="1900" windowWidth="25600" windowHeight="16060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>kolonner</t>
   </si>
@@ -36,23 +42,14 @@
     <t>antal kolonner pr søjle:</t>
   </si>
   <si>
-    <t>i alt</t>
-  </si>
-  <si>
     <t>0.5% i siderne, 1% gutter.  Dvs 0.5% på hver side af hver kolonne!</t>
-  </si>
-  <si>
-    <t>x3=</t>
-  </si>
-  <si>
-    <t>??</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -83,13 +80,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -101,7 +111,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="89">
+  <cellStyleXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -191,65 +201,71 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="89" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="1" fillId="2" borderId="0" xfId="89" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="89">
-    <cellStyle name="Besøgt link" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="88" builtinId="9" hidden="1"/>
+  <cellStyles count="90">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -295,9 +311,18 @@
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="89" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -622,24 +647,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -650,7 +675,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -658,47 +683,110 @@
         <v>3</v>
       </c>
       <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1">
+        <v>3</v>
+      </c>
+      <c r="F4" s="6">
+        <v>4</v>
+      </c>
+      <c r="G4" s="6">
         <v>5</v>
       </c>
-      <c r="D4" s="1">
-        <v>7</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>5</v>
+      <c r="H4" s="1">
+        <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>12</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3">
+        <f>1/A5</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C5" s="3">
+        <f>$B$5*C4</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D5" s="3">
+        <f>$B$5*D4</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E5" s="3">
+        <f>$B$5*E4</f>
+        <v>0.25</v>
+      </c>
+      <c r="F5" s="5">
+        <f>$B$5*F4</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G5" s="5">
+        <f>$B$5*G4</f>
+        <v>0.41666666666666663</v>
+      </c>
+      <c r="H5" s="3">
+        <f>$B$5*H4</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C7" s="7">
+        <v>7</v>
+      </c>
+      <c r="D7">
         <v>8</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>8</v>
+      <c r="E7">
+        <v>9</v>
+      </c>
+      <c r="F7">
+        <v>10</v>
+      </c>
+      <c r="G7">
+        <v>11</v>
+      </c>
+      <c r="H7" s="4">
+        <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
-      <c r="C7">
-        <v>4</v>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C8" s="5">
+        <f>$B$5*C7</f>
+        <v>0.58333333333333326</v>
+      </c>
+      <c r="D8" s="3">
+        <f>$B$5*D7</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E8" s="3">
+        <f>$B$5*E7</f>
+        <v>0.75</v>
+      </c>
+      <c r="F8" s="3">
+        <f>$B$5*F7</f>
+        <v>0.83333333333333326</v>
+      </c>
+      <c r="G8" s="3">
+        <f>$B$5*G7</f>
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="H8" s="5">
+        <f>$B$5*H7</f>
+        <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
-      <c r="C8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>8</v>
-      </c>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>